<commit_message>
feat: qa-level-1-planning-analysis.xlsx >> edit
</commit_message>
<xml_diff>
--- a/documents/qa-level-1-planning-analysis.xlsx
+++ b/documents/qa-level-1-planning-analysis.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>#</t>
   </si>
@@ -87,9 +87,6 @@
     <t>связи (# раздела, 999-все разделы)</t>
   </si>
   <si>
-    <t>инструкция (1-да, 0-нет)</t>
-  </si>
-  <si>
     <t>защищенность</t>
   </si>
   <si>
@@ -114,7 +111,25 @@
     <t>динамичный</t>
   </si>
   <si>
-    <t>динамичный (1-да, 0-нет)</t>
+    <t>кросс</t>
+  </si>
+  <si>
+    <t>логирование</t>
+  </si>
+  <si>
+    <t xml:space="preserve">установка </t>
+  </si>
+  <si>
+    <t>лицензии</t>
+  </si>
+  <si>
+    <t>функционал</t>
+  </si>
+  <si>
+    <t>структура</t>
+  </si>
+  <si>
+    <t>характеристика (1-да, 0-нет)</t>
   </si>
 </sst>
 </file>
@@ -187,27 +202,48 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+  <dxfs count="22">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -217,41 +253,6 @@
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -285,7 +286,18 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -301,28 +313,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:N12" totalsRowShown="0" headerRowDxfId="17">
-  <autoFilter ref="A1:N12"/>
-  <sortState ref="A2:N12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:T12" totalsRowShown="0" headerRowDxfId="19">
+  <autoFilter ref="A1:T12"/>
+  <sortState ref="A2:T12">
     <sortCondition descending="1" ref="F1:F12"/>
   </sortState>
-  <tableColumns count="14">
+  <tableColumns count="20">
     <tableColumn id="1" name="#" dataDxfId="18"/>
     <tableColumn id="2" name="раздел"/>
-    <tableColumn id="5" name="домен" dataDxfId="9"/>
-    <tableColumn id="6" name="связи" dataDxfId="8"/>
-    <tableColumn id="4" name="приоритет" dataDxfId="5"/>
-    <tableColumn id="14" name="рейтинг" dataDxfId="3">
+    <tableColumn id="5" name="домен" dataDxfId="17"/>
+    <tableColumn id="6" name="связи" dataDxfId="16"/>
+    <tableColumn id="4" name="приоритет" dataDxfId="15"/>
+    <tableColumn id="14" name="рейтинг" dataDxfId="14">
       <calculatedColumnFormula>SUM(Таблица1[[#This Row],[динамичный]:[локализация]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="динамичный" dataDxfId="4"/>
-    <tableColumn id="7" name="инструкция" dataDxfId="16"/>
-    <tableColumn id="8" name="защищенность" dataDxfId="15"/>
-    <tableColumn id="9" name="нагрузка" dataDxfId="14"/>
-    <tableColumn id="10" name="данные" dataDxfId="13"/>
-    <tableColumn id="11" name="адаптивность" dataDxfId="12"/>
-    <tableColumn id="12" name="доступность" dataDxfId="11"/>
-    <tableColumn id="13" name="локализация" dataDxfId="10"/>
+    <tableColumn id="3" name="динамичный" dataDxfId="13"/>
+    <tableColumn id="7" name="инструкция" dataDxfId="12"/>
+    <tableColumn id="20" name="структура" dataDxfId="11"/>
+    <tableColumn id="15" name="функционал" dataDxfId="10"/>
+    <tableColumn id="8" name="защищенность" dataDxfId="9"/>
+    <tableColumn id="9" name="нагрузка" dataDxfId="8"/>
+    <tableColumn id="10" name="данные" dataDxfId="7"/>
+    <tableColumn id="16" name="кросс" dataDxfId="6"/>
+    <tableColumn id="11" name="адаптивность" dataDxfId="5"/>
+    <tableColumn id="12" name="доступность" dataDxfId="4"/>
+    <tableColumn id="13" name="локализация" dataDxfId="3"/>
+    <tableColumn id="17" name="логирование" dataDxfId="2"/>
+    <tableColumn id="18" name="установка " dataDxfId="1"/>
+    <tableColumn id="19" name="лицензии" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -591,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,18 +625,21 @@
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -635,34 +656,52 @@
         <v>2</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="R1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -680,7 +719,7 @@
       </c>
       <c r="F2" s="4">
         <f>SUM(Таблица1[[#This Row],[динамичный]:[локализация]])</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -689,25 +728,41 @@
         <v>0</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
       </c>
       <c r="M2" s="1">
-        <v>0</v>
-      </c>
-      <c r="N2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -725,7 +780,7 @@
       </c>
       <c r="F3" s="4">
         <f>SUM(Таблица1[[#This Row],[динамичный]:[локализация]])</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -734,25 +789,41 @@
         <v>0</v>
       </c>
       <c r="I3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="1">
         <v>1</v>
       </c>
       <c r="M3" s="1">
-        <v>0</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>6</v>
       </c>
@@ -770,7 +841,7 @@
       </c>
       <c r="F4" s="4">
         <f>SUM(Таблица1[[#This Row],[динамичный]:[локализация]])</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G4" s="1">
         <v>1</v>
@@ -779,10 +850,10 @@
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="1">
         <v>0</v>
@@ -793,11 +864,27 @@
       <c r="M4" s="1">
         <v>0</v>
       </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N4" s="1"/>
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>10</v>
       </c>
@@ -833,21 +920,37 @@
         <v>0</v>
       </c>
       <c r="L5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5" s="1">
         <v>0</v>
       </c>
-      <c r="N5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N5" s="1"/>
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -860,7 +963,7 @@
       </c>
       <c r="F6" s="4">
         <f>SUM(Таблица1[[#This Row],[динамичный]:[локализация]])</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
@@ -869,7 +972,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="1">
         <v>0</v>
@@ -883,16 +986,32 @@
       <c r="M6" s="1">
         <v>0</v>
       </c>
-      <c r="N6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N6" s="1"/>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -901,20 +1020,20 @@
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" s="4">
         <f>SUM(Таблица1[[#This Row],[динамичный]:[локализация]])</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
       </c>
       <c r="I7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="1">
         <v>0</v>
@@ -928,16 +1047,32 @@
       <c r="M7" s="1">
         <v>0</v>
       </c>
-      <c r="N7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N7" s="1"/>
+      <c r="O7" s="1">
+        <v>1</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -973,16 +1108,32 @@
       <c r="M8" s="1">
         <v>0</v>
       </c>
-      <c r="N8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N8" s="1"/>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -991,14 +1142,14 @@
         <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" s="4">
         <f>SUM(Таблица1[[#This Row],[динамичный]:[локализация]])</f>
         <v>1</v>
       </c>
       <c r="G9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
@@ -1013,16 +1164,32 @@
         <v>0</v>
       </c>
       <c r="L9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="1">
         <v>0</v>
       </c>
-      <c r="N9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N9" s="1"/>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1040,7 +1207,7 @@
       </c>
       <c r="F10" s="4">
         <f>SUM(Таблица1[[#This Row],[динамичный]:[локализация]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
@@ -1049,7 +1216,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="1">
         <v>0</v>
@@ -1063,29 +1230,45 @@
       <c r="M10" s="1">
         <v>0</v>
       </c>
-      <c r="N10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N10" s="1"/>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
       <c r="D11" s="1">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="E11" s="1">
         <v>3</v>
       </c>
       <c r="F11" s="4">
         <f>SUM(Таблица1[[#This Row],[динамичный]:[локализация]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -1094,7 +1277,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="1">
         <v>0</v>
@@ -1108,22 +1291,38 @@
       <c r="M11" s="1">
         <v>0</v>
       </c>
-      <c r="N11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N11" s="1"/>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0</v>
+      </c>
+      <c r="T11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
       </c>
       <c r="D12" s="1">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="E12" s="1">
         <v>3</v>
@@ -1153,16 +1352,32 @@
       <c r="M12" s="1">
         <v>0</v>
       </c>
-      <c r="N12" s="1">
+      <c r="N12" s="1"/>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1">
+        <v>0</v>
+      </c>
+      <c r="T12" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:N12">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+  <conditionalFormatting sqref="G2:Q12">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1178,35 +1393,33 @@
   <dimension ref="B2:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>29</v>
+      <c r="B2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>19</v>
+      <c r="B5" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="B6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>